<commit_message>
Dataset used for sentiment analysis
</commit_message>
<xml_diff>
--- a/dataset.xlsx
+++ b/dataset.xlsx
@@ -5,16 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIYAL SOBTIPRIYAL.1\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PRIYAL SOBTIPRIYAL.1\Documents\mlproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E409CC10-6C61-40FC-B5E8-CD4E88A041EC}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FF4EEFB4-B027-48DE-8966-F55FFCF0C1D2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5652" xr2:uid="{DEDA7574-DAB7-4200-A6DA-4395A9F5D213}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="Sentiment">Sheet1!$A:$A</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,10 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Nice world</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>different</t>
   </si>
@@ -79,6 +79,24 @@
   </si>
   <si>
     <t>fab</t>
+  </si>
+  <si>
+    <t>Sentiment</t>
+  </si>
+  <si>
+    <t>Text</t>
+  </si>
+  <si>
+    <t>Neutral</t>
+  </si>
+  <si>
+    <t>positive</t>
+  </si>
+  <si>
+    <t>negative</t>
+  </si>
+  <si>
+    <t>neutral</t>
   </si>
 </sst>
 </file>
@@ -430,105 +448,163 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E2A95CD-8269-48E0-ADCB-91B5BF03D837}">
-  <dimension ref="A1:A18"/>
+  <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="B7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="B12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
+      <c r="B15" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
+      <c r="B17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>17</v>
+      <c r="B18" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>